<commit_message>
Cambié la organización de las importaciones y eliminé una función duplicada
Ahora todas las calls al cliente y la lógica termina en AI_functions.py
</commit_message>
<xml_diff>
--- a/data/output/CV_Sandra Popielarczyk_one_pager.xlsx
+++ b/data/output/CV_Sandra Popielarczyk_one_pager.xlsx
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SAP S/4HANA</t>
+          <t>CONTROL TOWER</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Data enthusiast with over 6 years of experience in transforming data into actionable insights. Specializes in gathering, processing, and analyzing information to support strategic goals. Currently enhancing **Python** and **SQL** skills to develop and optimize **Business Intelligence** solutions. Proven track record in data quality initiatives and automation projects that significantly improve team efficiency.</t>
+          <t>Data enthusiast with over 6 years of experience in transforming data into clear insights. Specializes in **gathering**, **processing**, and **analyzing** information to support strategic goals. Currently enhancing **Python** and **SQL** skills to develop Business Intelligence solutions. Proven track record in reducing document processing time by 50% and improving data reliability through quality initiatives.</t>
         </is>
       </c>
     </row>
@@ -504,7 +504,6 @@
       <c r="B6" t="inlineStr">
         <is>
           <t>Communications, Media &amp; Technology
-Financial Services
 Products</t>
         </is>
       </c>
@@ -563,8 +562,7 @@
           <t>Data Analyst  
 Responsible for **collecting** and **analyzing** data on public property in the Polish market, covering 800 companies.  
 Contributed to **automation projects** using **Python scripts** and **SQL queries** that reduced document processing time by 50%, optimizing workflows and boosting team efficiency.  
-Managed data quality initiatives by performing thorough **data validation** and **cleaning**, reducing errors and client-reported issues, which improved overall data reliability.  
-Developed and maintained interactive **Power BI reports** and dashboards to provide actionable insights for stakeholders and support **data-driven decision making**.</t>
+Developed and maintained interactive **Power BI reports** and dashboards to provide actionable insights for stakeholders and support data-driven decision making.</t>
         </is>
       </c>
     </row>
@@ -578,8 +576,7 @@
         <is>
           <t>International Forwarder  
 Managed and supervised **transportation logistics** for freight across multiple European countries, ensuring timely delivery and compliance with regulations.  
-Coordinated communication between clients, drivers, and warehouses to optimize **route planning** and resolve issues promptly.  
-Maintained accurate records and documentation for shipments, tracking status and ensuring all data was up to date.  
+Coordinated communication between clients, drivers, and warehouses to optimize route planning and resolve issues promptly.  
 Utilized **data tracking systems** to monitor shipment progress and identify opportunities to improve delivery efficiency.</t>
         </is>
       </c>

</xml_diff>